<commit_message>
data pages base 7-10
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases subs.xlsx
+++ b/src/com/data/Test Cases subs.xlsx
@@ -68,12 +68,33 @@
     <t>ConstructionFence</t>
   </si>
   <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>Antenna ::  :: I ::  :: approved :: 1000 ::  ::  :: rome18 ::  ::  :: exempted</t>
+  </si>
+  <si>
+    <t>user_info</t>
+  </si>
+  <si>
+    <t>AJOETEST2@GMAIL.COM :: Professional Engineer :: AJ2</t>
+  </si>
+  <si>
+    <t>CcSubs</t>
+  </si>
+  <si>
+    <t>AnSubs</t>
+  </si>
+  <si>
+    <t>DOBELECTRICIAN8@GMAIL.COM :: Electrician :: AJ2</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Subsequent Filing  - </t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -88,7 +109,37 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sprinklers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Subsequent Filing  - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>StandPipe</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Subsequent Filing  - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -103,7 +154,37 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CurbCut</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Subsequent Filing  - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sign</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Subsequent Filing  - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -118,52 +199,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Electrical</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Subsequent Filing  - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Sprinklers</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Subsequent Filing  - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CurbCut</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Subsequent Filing  - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
+        <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -173,7 +209,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -188,37 +224,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>StandPipe</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Subsequent Filing  - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Sign</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Subsequent Filing  - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
+        <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -228,32 +234,26 @@
     </r>
   </si>
   <si>
-    <t>filter</t>
-  </si>
-  <si>
-    <t>Antenna ::  :: I ::  :: approved :: 1000 ::  ::  :: rome18 ::  ::  :: exempted</t>
-  </si>
-  <si>
-    <t>user_info</t>
-  </si>
-  <si>
-    <t>AJOETEST2@GMAIL.COM :: Professional Engineer :: AJ2</t>
-  </si>
-  <si>
-    <t>CcSubs</t>
-  </si>
-  <si>
-    <t>AnSubs</t>
-  </si>
-  <si>
-    <t>DOBELECTRICIAN8@GMAIL.COM :: Electrician :: AJ2</t>
+    <r>
+      <t xml:space="preserve">Subsequent Filing  - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Electrical</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="27">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,28 +425,6 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -936,79 +914,10 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="34" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="35" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="38" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="38" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="38" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1021,6 +930,69 @@
     </xf>
     <xf numFmtId="49" fontId="23" fillId="34" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="34" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="38" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="38" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="128">
@@ -1458,9 +1430,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="35.140625" style="26" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="29" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="6" customWidth="1"/>
     <col min="4" max="16384" width="32.85546875" style="1"/>
   </cols>
   <sheetData>
@@ -1471,23 +1443,23 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="28" t="s">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="28" t="s">
+      <c r="A3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1501,620 +1473,528 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A22" sqref="A22:XFD32"/>
+      <selection pane="topRight" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="33.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="6" customWidth="1"/>
-    <col min="11" max="12" width="8.28515625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" style="7" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.5703125" style="7" customWidth="1"/>
-    <col min="21" max="21" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" style="7" customWidth="1"/>
-    <col min="23" max="23" width="10" style="7" customWidth="1"/>
-    <col min="24" max="28" width="14.85546875" style="7" customWidth="1"/>
-    <col min="29" max="29" width="15.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.85546875" style="7" customWidth="1"/>
-    <col min="32" max="32" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="22.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="18.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="3.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="22.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12" style="7" customWidth="1"/>
-    <col min="47" max="47" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="48" max="16384" width="27.140625" style="7"/>
+    <col min="1" max="1" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="54" style="11" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="33.140625" style="11"/>
+    <col min="15" max="16384" width="33.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="18" customFormat="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-    </row>
-    <row r="2" spans="1:14" s="18" customFormat="1">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-    </row>
-    <row r="3" spans="1:14" s="18" customFormat="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-    </row>
-    <row r="4" spans="1:14" s="18" customFormat="1">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-    </row>
-    <row r="5" spans="1:14" s="18" customFormat="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="25"/>
-    </row>
-    <row r="7" spans="1:14" s="18" customFormat="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-    </row>
-    <row r="8" spans="1:14" s="14" customFormat="1">
-      <c r="A8" s="5" t="s">
+    <row r="1" spans="1:14" s="8" customFormat="1">
+      <c r="B1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+    </row>
+    <row r="2" spans="1:14" s="8" customFormat="1">
+      <c r="B2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+    </row>
+    <row r="3" spans="1:14" s="8" customFormat="1">
+      <c r="B3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+    </row>
+    <row r="4" spans="1:14" s="8" customFormat="1">
+      <c r="B4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+    </row>
+    <row r="5" spans="1:14" s="8" customFormat="1">
+      <c r="B5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+    </row>
+    <row r="7" spans="1:14" s="8" customFormat="1">
+      <c r="B7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+    </row>
+    <row r="8" spans="1:14" s="16" customFormat="1">
+      <c r="A8" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" s="19" customFormat="1" ht="30">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="24" customFormat="1">
+      <c r="A10" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="24" customFormat="1">
+      <c r="A11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="24" customFormat="1">
+      <c r="A12" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="24" customFormat="1">
+      <c r="A13" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="24" customFormat="1">
+      <c r="A14" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="24" customFormat="1">
+      <c r="A15" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="24" customFormat="1">
+      <c r="A16" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="24" customFormat="1">
+      <c r="A17" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="24" customFormat="1">
+      <c r="A18" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-    </row>
-    <row r="9" spans="1:14" s="9" customFormat="1" ht="25.5">
-      <c r="A9" s="10" t="s">
+      <c r="C18" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="24" customFormat="1">
+      <c r="A19" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="25"/>
+    </row>
+    <row r="20" spans="1:6" s="26" customFormat="1">
+      <c r="B20" s="27"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+    </row>
+    <row r="21" spans="1:6" s="16" customFormat="1">
+      <c r="A21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" s="19" customFormat="1" ht="30">
+      <c r="A22" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B22" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C22" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="24" customFormat="1">
+      <c r="A23" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="24" customFormat="1">
+      <c r="A24" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="24" customFormat="1">
+      <c r="A25" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="24" customFormat="1">
+      <c r="A26" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="9" t="s">
+      <c r="C26" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="24" customFormat="1">
+      <c r="A27" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="24" customFormat="1">
+      <c r="A28" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="3" customFormat="1" ht="38.25">
-      <c r="A10" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="C28" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="24" customFormat="1">
+      <c r="A29" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="3" customFormat="1" ht="38.25">
-      <c r="A11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="3" customFormat="1" ht="38.25">
-      <c r="A12" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="3" customFormat="1" ht="38.25">
-      <c r="A13" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="13" t="s">
+      <c r="C29" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="3" customFormat="1" ht="38.25">
-      <c r="A14" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="3" customFormat="1" ht="38.25">
-      <c r="A15" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="3" customFormat="1" ht="38.25">
-      <c r="A16" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="24" t="s">
+      <c r="D29" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A17" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="13" t="s">
+      <c r="E29" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="24" customFormat="1">
+      <c r="A30" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="24" customFormat="1">
+      <c r="A31" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="24" customFormat="1">
+      <c r="A32" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A18" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A19" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" s="20" customFormat="1">
-      <c r="B20" s="21"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-    </row>
-    <row r="21" spans="1:6" s="14" customFormat="1">
-      <c r="A21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-    </row>
-    <row r="22" spans="1:6" s="9" customFormat="1" ht="25.5">
-      <c r="A22" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A23" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A24" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A25" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A26" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A27" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A28" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A29" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A30" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A31" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" ht="38.25">
-      <c r="A32" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="2:6" s="20" customFormat="1">
-      <c r="B33" s="21"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
+      <c r="F32" s="25"/>
+    </row>
+    <row r="33" spans="2:6" s="26" customFormat="1">
+      <c r="B33" s="27"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>